<commit_message>
push code báo cáo doanh số theo bus
</commit_message>
<xml_diff>
--- a/src/main/resources/template/report/Bao_cao_doanh_thu_hang_xe_theo_thoi_gian.xlsx
+++ b/src/main/resources/template/report/Bao_cao_doanh_thu_hang_xe_theo_thoi_gian.xlsx
@@ -3,19 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C2B67B-70E0-4969-9924-E988159F9B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9B225D-A487-48FC-849D-E5EDA33E8379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4056" yWindow="2940" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BC 6.2.4 aso_khong_hoat_dong" sheetId="2" r:id="rId1"/>
+    <sheet name="Báo cáo doanh thu theo hãng xe" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>&lt;jx:forEach items="${lstData}" var="vo" varStatus="status"&gt;</t>
   </si>
@@ -66,6 +66,30 @@
   </si>
   <si>
     <t>${vo.revenue}</t>
+  </si>
+  <si>
+    <t>Doanh số trước CK</t>
+  </si>
+  <si>
+    <t>Chiết khấu</t>
+  </si>
+  <si>
+    <t>${vo.discount}</t>
+  </si>
+  <si>
+    <t>${vo.ticketPrice}</t>
+  </si>
+  <si>
+    <t>Mã số xe</t>
+  </si>
+  <si>
+    <t>Mã loại xe</t>
+  </si>
+  <si>
+    <t>${vo.busCode}</t>
+  </si>
+  <si>
+    <t>${vo.typeBusCode}</t>
   </si>
 </sst>
 </file>
@@ -73,9 +97,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0\ &quot;VNĐ&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0\ &quot;VNĐ&quot;"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,21 +139,6 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="163"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="163"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -174,6 +183,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -264,14 +279,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -279,58 +291,53 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,6 +353,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{789513BC-D0A9-09E1-C32D-C828961C0AF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38100" y="68580"/>
+          <a:ext cx="2712720" cy="1089660"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -635,192 +691,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A4:S12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" style="22" customWidth="1"/>
-    <col min="5" max="5" width="27.21875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16" style="5" customWidth="1"/>
-    <col min="7" max="7" width="23.88671875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" style="5" customWidth="1"/>
-    <col min="9" max="11" width="20.33203125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="14.77734375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="22.6640625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="34" style="5" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="5"/>
+    <col min="1" max="1" width="9.77734375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="17" style="4" customWidth="1"/>
+    <col min="6" max="7" width="21" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" style="19" customWidth="1"/>
+    <col min="9" max="9" width="27.21875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="16" style="4" customWidth="1"/>
+    <col min="11" max="11" width="23.88671875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" style="4" customWidth="1"/>
+    <col min="13" max="15" width="20.33203125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="14.77734375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="22.6640625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="34" style="4" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="4" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+    </row>
+    <row r="5" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="E6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="G6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+    <row r="7" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+    <row r="8" spans="1:19" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="F8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
     </row>
-    <row r="5" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+    <row r="9" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="24"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5" s="17"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="21"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9" s="14"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
     </row>
-    <row r="6" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+    <row r="10" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="F10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
     </row>
-    <row r="7" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+    <row r="11" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="24"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7" s="17"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="21"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11" s="14"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
     </row>
-    <row r="8" spans="1:15" s="18" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+    <row r="12" spans="1:19" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="H12" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>